<commit_message>
did that one man ask
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -382,10 +382,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>hello</v>
+        <v>kjedshgfsajd</v>
       </c>
       <c r="B1" t="str">
-        <v>world</v>
+        <v>workjHADJKHJKld</v>
       </c>
     </row>
   </sheetData>

</xml_diff>